<commit_message>
Some bug fixes from Michael
</commit_message>
<xml_diff>
--- a/files for logic.xlsx
+++ b/files for logic.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>admin.html</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>my details only if logged in AND did not attend</t>
   </si>
 </sst>
 </file>
@@ -166,8 +169,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -213,6 +220,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -226,6 +235,8 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -719,7 +730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="B17" t="s">
         <v>19</v>
       </c>
@@ -730,7 +741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -738,70 +749,91 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="B26" t="s">
         <v>19</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="B28" t="s">
         <v>28</v>
       </c>
@@ -809,7 +841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:6">
       <c r="B29" t="s">
         <v>29</v>
       </c>

</xml_diff>